<commit_message>
Update effort log and add diagrams for sprint 2 submission Update effort log to include detailed information outlining my most recent efforts. Also, create a diagrams folder that contains use case diagram, domain class diagram, and design class diagram. Lastly, add sprint 1 and sprint 2 Power Point presetations. This commit ensures my branch is up-to-date with our teams most recent changes and efforts.
</commit_message>
<xml_diff>
--- a/docs/efforts/Travis Thayer.xlsx
+++ b/docs/efforts/Travis Thayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onebe\Documents\Oakland University\CSI_4999\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89678760-EC08-4336-8198-870DCF0E9641}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304EC260-41BA-488D-999E-AC68F535EDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>Established communication via Discord, scheduled team meetings, created Power Point presentation, and proposed configuration management options.</t>
+  </si>
+  <si>
+    <t>UseCaseDiagram.mdj; DomainClassDiagram.mdj; GCP (gptms-vm)</t>
+  </si>
+  <si>
+    <t>Setup Bitnami LAMP stack on GCP virtual machine, and installed Python and Flask. Configured SSH keys for back-end team and created secure tunnel for access to phpmyadmin. Created the Use Case Diagram and also the Domain Class Diagram based on the Base Diagram. Lastly, I helped schedule our team meetings.</t>
+  </si>
+  <si>
+    <t>https://github.com/quentinxs/GPTMS/tree/travis/docs/diagrams; https://github.com/quentinxs/GPTMS/tree/travis/docs/presentations; 34.70.164.45; Discord</t>
+  </si>
+  <si>
+    <t>3, 5, 6[IT], 6[CS]</t>
+  </si>
+  <si>
+    <t>Sprint2.pptx; UseCaseDiagram.mdj; DomainClassDiagram.mdj; GCP (34.70.164.45)</t>
   </si>
 </sst>
 </file>
@@ -291,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -317,21 +332,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -344,24 +368,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -373,6 +379,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -667,46 +685,46 @@
     <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="38.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="16" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
@@ -727,163 +745,180 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="13">
+      <c r="B4" s="13"/>
+      <c r="C4" s="27">
         <v>16</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="11">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -897,11 +932,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -925,47 +955,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1029,28 +1059,28 @@
       <c r="A6" s="7">
         <v>1</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>0</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>0</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <v>0</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="11">
         <v>1</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>0</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update efforts for Sprint 3
</commit_message>
<xml_diff>
--- a/docs/efforts/Travis Thayer.xlsx
+++ b/docs/efforts/Travis Thayer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onebe\Documents\Oakland University\CSI_4999\GPTMS\docs\efforts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005FFDC2-C49F-490B-A994-CDC9DF9A8306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC591ABF-313D-4E65-ADEA-D47CC1C6A68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Sprint2.pptx; UseCaseDiagram.mdj; DomainClassDiagram.mdj; GCP (34.70.164.45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switched from Python/Flask to PHP/Apache for easier MVC integration. Created an endpoint for the login page and registration page. Created a User class, user controller, SQL connection via mysqli, and related SQL queries for login and registration funtionality. </t>
+  </si>
+  <si>
+    <t>profileController.php; ProfileQueries.php; databaseConnection.php; User.php</t>
+  </si>
+  <si>
+    <t>https://github.com/quentinxs/GPTMS/blob/travis/api/User/User.php; https://github.com/quentinxs/GPTMS/blob/travis/api/User/profileController.php; https://github.com/quentinxs/GPTMS/blob/travis/api/User/profileQueries.php</t>
   </si>
 </sst>
 </file>
@@ -346,6 +355,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -356,24 +383,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -670,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -687,40 +696,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
@@ -741,10 +750,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="11">
         <v>16</v>
       </c>
@@ -765,10 +774,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="9">
         <v>16</v>
       </c>
@@ -788,23 +797,35 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="9">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
@@ -813,10 +834,10 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
@@ -825,10 +846,10 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
@@ -837,10 +858,10 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
@@ -849,10 +870,10 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
@@ -861,10 +882,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
@@ -873,10 +894,10 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
@@ -885,10 +906,10 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
@@ -897,10 +918,10 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
@@ -910,6 +931,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -923,11 +949,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -937,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -966,19 +987,19 @@
       <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25"/>
@@ -1113,14 +1134,30 @@
       <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">

</xml_diff>

<commit_message>
Update effort log for Sprint4
</commit_message>
<xml_diff>
--- a/docs/efforts/Travis Thayer.xlsx
+++ b/docs/efforts/Travis Thayer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC591ABF-313D-4E65-ADEA-D47CC1C6A68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC900955-291C-483D-8299-F0F24A768D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>https://github.com/quentinxs/GPTMS/blob/travis/api/User/User.php; https://github.com/quentinxs/GPTMS/blob/travis/api/User/profileController.php; https://github.com/quentinxs/GPTMS/blob/travis/api/User/profileQueries.php</t>
+  </si>
+  <si>
+    <t>userController.php; userQueries.php; profile.php; .htaccess;  README.md; 404.php; courseController.php; courseQueries.php</t>
+  </si>
+  <si>
+    <t>https://github.com/quentinxs/GPTMS/tree/travis/api/courses/*; https://github.com/quentinxs/GPTMS/tree/travis/api/errors/*; https://github.com/quentinxs/GPTMS/tree/travis/api/users/*</t>
+  </si>
+  <si>
+    <t>Created two controllers for the users and courses collections (endpoints). Created services and sub-services for the users and courses collections. Created corresponding functions for services that are used to query the database via mysqli. Programmmed proper http method and data validation and filtering; along with SQL parameterization. Created .htaccess files for directory navigation and custom error caching. Created README.md files for each collection/service.</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5, 6[CS]</t>
   </si>
 </sst>
 </file>
@@ -315,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -396,6 +408,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -821,17 +836,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="15"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="C7" s="9">
+        <v>24</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
@@ -959,7 +986,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1163,14 +1190,30 @@
       <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">

</xml_diff>

<commit_message>
Update Effort Workbook for Sprint 5
</commit_message>
<xml_diff>
--- a/docs/efforts/Travis Thayer.xlsx
+++ b/docs/efforts/Travis Thayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC900955-291C-483D-8299-F0F24A768D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC4C0DB-D16E-4CD2-839B-93C0170ED7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>2, 3, 4, 5, 6[CS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added a document resource and to all URIs and expanded on URI path naming validation. Updated all the README.md files in api directory. Wrote the controller logic and SQL queries to update and/or delete an existing user profile. Adjusted relationships and added a Tee table to ERD in-order to better accomidate the number of tees available per course. Adusted relationships in the ERD pertaining to a player's score to allow tracking a player's score per hole per course. Changed Role table to Employee table to narrow the project scope. Created a new data insertion and database creation script for the newly updated ERD. Added a code of conduct to the project documentation. </t>
+  </si>
+  <si>
+    <t>userMngmtController.php; README.md (3 total); courseMngmtController.php; userMngmtQueries.php; courseMngmtQueries.php; GPTMS-ERD.mwb; Database_Data_Insertion_Script.sql; Database_Creation_Script.sql; .gitignore; CODE_OF_CONDUCT.md</t>
+  </si>
+  <si>
+    <t>https://github.com/quentinxs/GPTMS/tree/travis/api/user-management/*; https://github.com/quentinxs/GPTMS/tree/travis/api/course-management/*; https://github.com/quentinxs/GPTMS/blob/travis/api/README.md; https://github.com/quentinxs/GPTMS/blob/travis/CODE_OF_CONDUCT.md; https://github.com/quentinxs/GPTMS/blob/travis/api/database-management/Database_Creation_Script.sql; https://github.com/quentinxs/GPTMS/blob/travis/api/database-management/Database_Data_Insertion_Script.sql; https://github.com/quentinxs/GPTMS/blob/travis/api/database-management/GPTMS-ERD.mwb</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5, 6[IT]</t>
   </si>
 </sst>
 </file>
@@ -367,6 +379,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -385,18 +412,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -408,9 +423,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -705,46 +717,46 @@
     <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="6" max="6" width="25.19921875" customWidth="1"/>
     <col min="7" max="7" width="38.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
@@ -765,10 +777,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="11">
         <v>16</v>
       </c>
@@ -789,10 +801,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="9">
         <v>16</v>
       </c>
@@ -813,10 +825,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="9">
         <v>16</v>
       </c>
@@ -837,10 +849,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="9">
         <v>24</v>
       </c>
@@ -853,30 +865,42 @@
       <c r="F7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="15" t="s">
         <v>44</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:8" ht="280.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="9">
+        <v>24</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
@@ -885,10 +909,10 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
@@ -897,10 +921,10 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
@@ -909,10 +933,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
@@ -921,10 +945,10 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
@@ -933,10 +957,10 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
@@ -945,10 +969,10 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
@@ -958,11 +982,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -976,6 +995,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -985,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -999,47 +1023,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1219,14 +1243,30 @@
       <c r="A10" s="5">
         <v>5</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">

</xml_diff>

<commit_message>
Update work effort log
</commit_message>
<xml_diff>
--- a/docs/efforts/Travis Thayer.xlsx
+++ b/docs/efforts/Travis Thayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC4C0DB-D16E-4CD2-839B-93C0170ED7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA320FC-D28A-4C20-9EA5-95ABDA29CFCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -182,6 +182,18 @@
   </si>
   <si>
     <t>2, 3, 4, 5, 6[IT]</t>
+  </si>
+  <si>
+    <t>2, 3, 4</t>
+  </si>
+  <si>
+    <t>Added URIs for the party management document to manage a players score. Updated ERD to include a hints entity that relates to course. Fixed the history queries. Created URIs for returning all active parties and created URI for returning all course, hole, and tee data.</t>
+  </si>
+  <si>
+    <t>PartyMngmtController.php; PartyMngmtQueries.php; GPTMS-ERD.mwb; userMngmtQueries.php;  userMngmtController.php</t>
+  </si>
+  <si>
+    <t>https://github.com/quentinxs/GPTMS/tree/travis/api/party-management/*; https://github.com/quentinxs/GPTMS/tree/travis/api/user-management/*; https://github.com/quentinxs/GPTMS/blob/travis/api/database-management/GPTMS-ERD.mwb</t>
   </si>
 </sst>
 </file>
@@ -339,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -382,6 +394,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,24 +424,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,6 +435,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -723,40 +738,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
@@ -777,10 +792,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="11">
         <v>16</v>
       </c>
@@ -801,10 +816,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="9">
         <v>16</v>
       </c>
@@ -825,10 +840,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="9">
         <v>16</v>
       </c>
@@ -849,10 +864,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="9">
         <v>24</v>
       </c>
@@ -873,10 +888,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="280.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="9">
         <v>24</v>
       </c>
@@ -896,23 +911,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="9">
+        <v>24</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
@@ -921,10 +948,10 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
@@ -933,10 +960,10 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="20"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
@@ -945,10 +972,10 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
@@ -957,10 +984,10 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
@@ -969,10 +996,10 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
@@ -982,6 +1009,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -995,11 +1027,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1009,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1038,19 +1065,19 @@
       <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
@@ -1272,14 +1299,30 @@
       <c r="A11" s="5">
         <v>6</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">

</xml_diff>